<commit_message>
Signed-off-by sig at mairie-avignon.com le 25/01/2022  0:41:25,92
</commit_message>
<xml_diff>
--- a/84007-parcsJardins-20220124/metadata/84007-parcsJardins-20220124-metadata-openpaca.xlsx
+++ b/84007-parcsJardins-20220124/metadata/84007-parcsJardins-20220124-metadata-openpaca.xlsx
@@ -6,14 +6,15 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="84007-parcsJardins-20220124-met" sheetId="1" r:id="rId2"/>
+    <sheet name="84007-parcsJardins-20220124-met" sheetId="2" r:id="rId4"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
   <si>
     <t/>
   </si>
@@ -131,7 +132,7 @@
     <numFmt numFmtId="167" formatCode="h:mm:ss AM/PM"/>
     <numFmt numFmtId="168" formatCode="mmm dd, yyyy h:mm:ss AM/PM"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -141,6 +142,42 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <sz val="12"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <b/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
@@ -157,7 +194,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -167,17 +204,47 @@
     </border>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true">
       <alignment wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="true">
       <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -186,172 +253,172 @@
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B20"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" style="1" customWidth="true"/>
-    <col min="2" max="2" width="80.7109375" style="2" customWidth="true"/>
+    <col min="1" max="1" width="40.7109375" style="3" customWidth="true"/>
+    <col min="2" max="2" width="80.7109375" style="4" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="A19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="6" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>